<commit_message>
added customer management file
</commit_message>
<xml_diff>
--- a/order_history_2025-03-08.xlsx
+++ b/order_history_2025-03-08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,7 +606,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Delivered</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Not Paid</t>
+          <t>Paid</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -922,6 +922,41 @@
       <c r="G14" t="inlineStr">
         <is>
           <t>Pending</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>20250308004312</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-03-08 00:43:12</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>[{'Item Name': 'Roti Sabzi', 'Price': 100.0}]</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>100</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Take Away</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Delivered</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
kinda everything works now
</commit_message>
<xml_diff>
--- a/order_history_2025-03-08.xlsx
+++ b/order_history_2025-03-08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -960,6 +960,41 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>20250308110347</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2025-03-08 11:03:47</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>[{'Item Name': 'Veg Thali', 'Price': 150.0}, {'Item Name': 'Roti Sabzi', 'Price': 100.0}, {'Item Name': 'Veg Thali', 'Price': 150.0}]</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>400</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Take Away</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
order type filter applied and title changed to marathi font
</commit_message>
<xml_diff>
--- a/order_history_2025-03-08.xlsx
+++ b/order_history_2025-03-08.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -635,6 +635,166 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>20250308000711</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-03-08 00:07:11</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>[{'Item Name': 'Veg Thali', 'Price': 150.0}]</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>150</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Take Away</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>20250308000718</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-03-08 00:07:18</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>[{'Item Name': 'Dal Rice', 'Price': 120.0}]</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>120</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Paid</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Take Away</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>20250308155356</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-03-08 15:53:56</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>[{'Item Name': 'South Indian Thali', 'Price': 200.0}, {'Item Name': 'South Indian Thali', 'Price': 200.0}]</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>400</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Not Paid</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Take Away</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>20250308155419</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-03-08 15:54:19</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>[{'Item Name': 'Veg Thali', 'Price': 150.0}, {'Item Name': 'Roti Sabzi', 'Price': 100.0}, {'Item Name': 'Roti Sabzi', 'Price': 100.0}, {'Item Name': 'Roti Sabzi', 'Price': 100.0}]</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>450</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Not Paid</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Take Away</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>rajas 1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>